<commit_message>
Changes made to handle atomized inputs/outputs and changes to display to better highlight param/performer additions and db_id entries.
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/gus/GusAppFramework/branches/4.0@13051 4235af6a-31f9-0310-9ad3-ecf6348f2534
</commit_message>
<xml_diff>
--- a/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx3.xlsx
+++ b/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-7635" yWindow="2415" windowWidth="19440" windowHeight="8085" tabRatio="162" activeTab="1"/>
@@ -10,7 +10,7 @@
     <sheet name="IDF" sheetId="1" r:id="rId1"/>
     <sheet name="SDRF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -755,9 +755,6 @@
     <t>COND 1 -3 cov</t>
   </si>
   <si>
-    <t>COND 0 -1 quant</t>
-  </si>
-  <si>
     <t>COND 0 -2 quant</t>
   </si>
   <si>
@@ -770,9 +767,6 @@
     <t>COND 1 -2 quant</t>
   </si>
   <si>
-    <t>COND 1 -3 quant</t>
-  </si>
-  <si>
     <t>Comment [ExtDbRls]</t>
   </si>
   <si>
@@ -927,12 +921,18 @@
   </si>
   <si>
     <t>NEW PROT 4</t>
+  </si>
+  <si>
+    <t>COND 0 -1 quant &lt;id=q1&gt;</t>
+  </si>
+  <si>
+    <t>COND 1 -3 quant &lt;id=q3&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="41">
     <font>
       <sz val="11"/>
@@ -1941,7 +1941,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1976,7 +1975,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2152,7 +2150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2188,10 +2186,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="73" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="60">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
@@ -2329,7 +2327,7 @@
         <v>108</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:256">
@@ -3603,7 +3601,7 @@
         <v>110</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>70</v>
@@ -3621,16 +3619,16 @@
         <v>54</v>
       </c>
       <c r="I39" s="64" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J39" s="64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K39" s="64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L39" s="64" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M39" s="35"/>
       <c r="N39" s="35"/>
@@ -3791,16 +3789,16 @@
         <v>191</v>
       </c>
       <c r="I42" s="64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J42" s="64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K42" s="64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L42" s="64" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="M42" s="35"/>
       <c r="N42" s="35"/>
@@ -3956,16 +3954,16 @@
         <v>0</v>
       </c>
       <c r="I45" s="64" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J45" s="64" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K45" s="64" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L45" s="64" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M45" s="35"/>
       <c r="N45" s="35"/>
@@ -4163,10 +4161,10 @@
         <v>164</v>
       </c>
       <c r="J49" s="64" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K49" s="64" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="L49" s="72"/>
       <c r="M49" s="35"/>
@@ -4248,13 +4246,13 @@
         <v>187</v>
       </c>
       <c r="I54" s="67" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J54" s="66" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K54" s="66" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:41">
@@ -4328,11 +4326,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:EG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BK16" sqref="BK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4387,10 +4385,10 @@
         <v>188</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E1" s="46" t="s">
         <v>29</v>
@@ -4420,7 +4418,7 @@
         <v>107</v>
       </c>
       <c r="N1" s="47" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="O1" s="48" t="s">
         <v>33</v>
@@ -4456,7 +4454,7 @@
         <v>32</v>
       </c>
       <c r="Z1" s="48" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AA1" s="48" t="s">
         <v>32</v>
@@ -4519,7 +4517,7 @@
         <v>227</v>
       </c>
       <c r="AU1" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AV1" s="46" t="s">
         <v>32</v>
@@ -4540,7 +4538,7 @@
         <v>35</v>
       </c>
       <c r="BB1" s="47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="BC1" s="51" t="s">
         <v>42</v>
@@ -4579,16 +4577,16 @@
         <v>239</v>
       </c>
       <c r="BO1" s="51" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="BP1" s="48" t="s">
         <v>106</v>
       </c>
       <c r="BQ1" s="46" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="BR1" s="46" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:137" ht="15.75">
@@ -4599,10 +4597,10 @@
         <v>210</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>253</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>255</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>196</v>
@@ -4614,7 +4612,7 @@
         <v>38</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>112</v>
@@ -4650,7 +4648,7 @@
         <v>112</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U2" s="30" t="s">
         <v>144</v>
@@ -4726,7 +4724,7 @@
         <v>33</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>213</v>
@@ -4774,28 +4772,28 @@
         <v>219</v>
       </c>
       <c r="BK2" s="4" t="s">
-        <v>246</v>
+        <v>302</v>
       </c>
       <c r="BL2" s="56" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="BM2" s="56" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="BN2" s="56" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="BO2" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP2" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ2" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR2" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:137" s="63" customFormat="1" ht="15.75">
@@ -4806,10 +4804,10 @@
         <v>210</v>
       </c>
       <c r="C3" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="74" t="s">
         <v>253</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>255</v>
       </c>
       <c r="E3" s="74" t="s">
         <v>196</v>
@@ -4821,7 +4819,7 @@
         <v>38</v>
       </c>
       <c r="H3" s="74" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I3" s="74" t="s">
         <v>112</v>
@@ -4857,7 +4855,7 @@
         <v>112</v>
       </c>
       <c r="T3" s="76" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U3" s="74" t="s">
         <v>144</v>
@@ -4933,13 +4931,13 @@
         <v>33</v>
       </c>
       <c r="AT3" s="74" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AU3" s="56" t="s">
         <v>213</v>
       </c>
       <c r="AV3" s="61" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AW3" s="61" t="s">
         <v>145</v>
@@ -4949,13 +4947,13 @@
       <c r="AZ3" s="71"/>
       <c r="BA3" s="56"/>
       <c r="BB3" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="BC3" s="56" t="s">
+        <v>294</v>
+      </c>
+      <c r="BD3" s="56" t="s">
         <v>280</v>
-      </c>
-      <c r="BC3" s="56" t="s">
-        <v>296</v>
-      </c>
-      <c r="BD3" s="56" t="s">
-        <v>282</v>
       </c>
       <c r="BE3" s="56" t="s">
         <v>54</v>
@@ -4973,31 +4971,31 @@
         <v>75</v>
       </c>
       <c r="BJ3" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="BK3" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="BL3" s="56" t="s">
+        <v>301</v>
+      </c>
+      <c r="BM3" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="BK3" s="56" t="s">
-        <v>299</v>
-      </c>
-      <c r="BL3" s="56" t="s">
-        <v>303</v>
-      </c>
-      <c r="BM3" s="56" t="s">
-        <v>300</v>
-      </c>
       <c r="BN3" s="56" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="BO3" s="56" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP3" s="56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ3" s="56" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR3" s="56" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="BS3" s="56"/>
       <c r="BT3" s="56"/>
@@ -5068,10 +5066,10 @@
         <v>211</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>196</v>
@@ -5083,7 +5081,7 @@
         <v>38</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>112</v>
@@ -5119,7 +5117,7 @@
         <v>112</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U4" s="30" t="s">
         <v>144</v>
@@ -5243,22 +5241,22 @@
         <v>220</v>
       </c>
       <c r="BK4" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BL4" s="56"/>
       <c r="BM4" s="56"/>
       <c r="BN4" s="56"/>
       <c r="BO4" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP4" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ4" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR4" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:137" ht="15.75">
@@ -5269,10 +5267,10 @@
         <v>212</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>196</v>
@@ -5284,7 +5282,7 @@
         <v>38</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>112</v>
@@ -5320,7 +5318,7 @@
         <v>112</v>
       </c>
       <c r="T5" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U5" s="30" t="s">
         <v>144</v>
@@ -5444,22 +5442,22 @@
         <v>221</v>
       </c>
       <c r="BK5" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BL5" s="56"/>
       <c r="BM5" s="56"/>
       <c r="BN5" s="56"/>
       <c r="BO5" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP5" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ5" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR5" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:137" ht="15.75">
@@ -5470,10 +5468,10 @@
         <v>63</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>196</v>
@@ -5485,7 +5483,7 @@
         <v>38</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>112</v>
@@ -5521,7 +5519,7 @@
         <v>112</v>
       </c>
       <c r="T6" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U6" s="30" t="s">
         <v>144</v>
@@ -5647,22 +5645,22 @@
         <v>76</v>
       </c>
       <c r="BK6" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BL6" s="56"/>
       <c r="BM6" s="56"/>
       <c r="BN6" s="56"/>
       <c r="BO6" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP6" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ6" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR6" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:137" ht="15.75">
@@ -5673,10 +5671,10 @@
         <v>64</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>254</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>256</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>196</v>
@@ -5688,7 +5686,7 @@
         <v>38</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>112</v>
@@ -5724,7 +5722,7 @@
         <v>112</v>
       </c>
       <c r="T7" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U7" s="30" t="s">
         <v>144</v>
@@ -5850,22 +5848,22 @@
         <v>77</v>
       </c>
       <c r="BK7" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BL7" s="56"/>
       <c r="BM7" s="56"/>
       <c r="BN7" s="56"/>
       <c r="BO7" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP7" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ7" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR7" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:137" ht="15.75">
@@ -5876,10 +5874,10 @@
         <v>65</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>196</v>
@@ -5891,7 +5889,7 @@
         <v>38</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>112</v>
@@ -5927,7 +5925,7 @@
         <v>112</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="V8" s="4" t="s">
         <v>82</v>
@@ -6050,36 +6048,36 @@
         <v>78</v>
       </c>
       <c r="BK8" s="4" t="s">
-        <v>251</v>
+        <v>303</v>
       </c>
       <c r="BL8" s="56" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="BM8" s="56" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="BN8" s="56" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="BO8" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP8" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ8" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR8" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:137" s="63" customFormat="1" ht="15.75">
       <c r="A9" s="56" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C9" s="56"/>
       <c r="D9" s="56"/>
@@ -6093,7 +6091,7 @@
         <v>38</v>
       </c>
       <c r="H9" s="56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I9" s="56" t="s">
         <v>112</v>
@@ -6105,16 +6103,16 @@
         <v>224</v>
       </c>
       <c r="L9" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="M9" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="N9" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="M9" s="56" t="s">
+      <c r="O9" s="56" t="s">
         <v>272</v>
-      </c>
-      <c r="N9" s="56" t="s">
-        <v>273</v>
-      </c>
-      <c r="O9" s="56" t="s">
-        <v>274</v>
       </c>
       <c r="P9" s="56" t="s">
         <v>39</v>
@@ -6129,13 +6127,13 @@
         <v>112</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U9" s="56" t="s">
         <v>144</v>
       </c>
       <c r="V9" s="56" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="W9" s="56" t="s">
         <v>197</v>
@@ -6150,7 +6148,7 @@
         <v>10</v>
       </c>
       <c r="AA9" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AC9" s="56"/>
       <c r="AD9" s="56"/>
@@ -6167,7 +6165,7 @@
         <v>101</v>
       </c>
       <c r="AI9" s="56" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AJ9" s="60" t="s">
         <v>177</v>
@@ -6200,13 +6198,13 @@
         <v>33</v>
       </c>
       <c r="AT9" s="56" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AU9" s="56" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AV9" s="61" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AW9" s="61" t="s">
         <v>145</v>
@@ -6214,13 +6212,13 @@
       <c r="AZ9" s="56"/>
       <c r="BA9" s="62"/>
       <c r="BB9" s="61" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="BC9" s="56" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="BD9" s="56" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="BE9" s="56" t="s">
         <v>54</v>
@@ -6232,34 +6230,34 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="BH9" s="56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="BI9" s="56" t="s">
         <v>75</v>
       </c>
       <c r="BJ9" s="56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="BK9" s="56" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="BL9" s="56" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="BM9" s="56" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="BN9" s="56" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="BO9" s="56" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="BP9" s="56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BQ9" s="56" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BR9" s="63">
         <v>2</v>

</xml_diff>